<commit_message>
Implement symbolic regression models
</commit_message>
<xml_diff>
--- a/performance_data/trained/test/metrics.xlsx
+++ b/performance_data/trained/test/metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,37 +456,57 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>rmse_vcell_hybrid_without_delta [mV]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>rmse_vcell_rom [mV]</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>rmse_thetass2_spme [milli]</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>rmse_thetass2_hybrid [milli]</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_thetass2_hybrid_without_delta [milli]</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>rmse_phie2_spme [mV]</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>rmse_phie2_hybrid [mV]</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_phie2_hybrid_without_delta [mV]</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>rmse_if2_spme [mA]</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>rmse_if2_hybrid [mA]</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_if2_hybrid_without_delta [mA]</t>
         </is>
       </c>
     </row>
@@ -508,26 +528,38 @@
         <v>18.78470331533877</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5010830831818629</v>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="n">
+        <v>0.2484402900329776</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.41983471626149</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
         <v>43.7358703437796</v>
       </c>
-      <c r="H2" t="n">
-        <v>0.1822110225073381</v>
-      </c>
       <c r="I2" t="n">
+        <v>0.267014520436426</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.996485785104415</v>
+      </c>
+      <c r="K2" t="n">
         <v>2.978995576824035</v>
       </c>
-      <c r="J2" t="n">
-        <v>0.202168528013874</v>
-      </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
+        <v>0.1915680168484054</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.9584283649439964</v>
+      </c>
+      <c r="N2" t="n">
         <v>56.67263062870067</v>
       </c>
-      <c r="L2" t="n">
-        <v>10.38990987723403</v>
+      <c r="O2" t="n">
+        <v>1.986758250353938</v>
+      </c>
+      <c r="P2" t="n">
+        <v>4.853599605237231</v>
       </c>
     </row>
     <row r="3">
@@ -548,26 +580,38 @@
         <v>5.003483852125205</v>
       </c>
       <c r="E3" t="n">
-        <v>0.06846654489863928</v>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
+        <v>0.1992275861903888</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.683943637335505</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
         <v>15.034764981421</v>
       </c>
-      <c r="H3" t="n">
-        <v>0.1831979906680053</v>
-      </c>
       <c r="I3" t="n">
+        <v>0.2291191651059691</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.50508416648509</v>
+      </c>
+      <c r="K3" t="n">
         <v>0.2532317906993753</v>
       </c>
-      <c r="J3" t="n">
-        <v>0.07565750108012075</v>
-      </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
+        <v>0.1094559105373297</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.2673031981268261</v>
+      </c>
+      <c r="N3" t="n">
         <v>5.177685837604972</v>
       </c>
-      <c r="L3" t="n">
-        <v>2.232719620978559</v>
+      <c r="O3" t="n">
+        <v>0.5981098243075972</v>
+      </c>
+      <c r="P3" t="n">
+        <v>12.18018861377182</v>
       </c>
     </row>
     <row r="4">
@@ -588,26 +632,38 @@
         <v>4.839307579931836</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3214365846734404</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
+        <v>0.2957377338123012</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.272985895707731</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="n">
         <v>14.87308574524844</v>
       </c>
-      <c r="H4" t="n">
-        <v>0.2939603887173026</v>
-      </c>
       <c r="I4" t="n">
+        <v>0.3188370031423483</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2.969493742516178</v>
+      </c>
+      <c r="K4" t="n">
         <v>0.4996402611546773</v>
       </c>
-      <c r="J4" t="n">
-        <v>0.1091391136828821</v>
-      </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
+        <v>0.1195641350490709</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1.362948717325113</v>
+      </c>
+      <c r="N4" t="n">
         <v>9.120512990525478</v>
       </c>
-      <c r="L4" t="n">
-        <v>1.432670825226723</v>
+      <c r="O4" t="n">
+        <v>1.005707166316514</v>
+      </c>
+      <c r="P4" t="n">
+        <v>21.53801454238877</v>
       </c>
     </row>
     <row r="5">
@@ -628,26 +684,38 @@
         <v>17.3959451475703</v>
       </c>
       <c r="E5" t="n">
-        <v>1.225399141718276</v>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="n">
+        <v>4.062989119600359</v>
+      </c>
+      <c r="F5" t="n">
+        <v>7.638299160277519</v>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="n">
         <v>46.71988130681122</v>
       </c>
-      <c r="H5" t="n">
-        <v>0.5758731939780444</v>
-      </c>
       <c r="I5" t="n">
+        <v>3.194834529683527</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5.731017690657275</v>
+      </c>
+      <c r="K5" t="n">
         <v>4.142925913006523</v>
       </c>
-      <c r="J5" t="n">
-        <v>0.3506250483337384</v>
-      </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
+        <v>0.2663234867236759</v>
+      </c>
+      <c r="M5" t="n">
+        <v>5.830591755813333</v>
+      </c>
+      <c r="N5" t="n">
         <v>77.16998448259233</v>
       </c>
-      <c r="L5" t="n">
-        <v>2.950767038192517</v>
+      <c r="O5" t="n">
+        <v>3.037047053381891</v>
+      </c>
+      <c r="P5" t="n">
+        <v>11.25843421902136</v>
       </c>
     </row>
     <row r="6">
@@ -668,26 +736,38 @@
         <v>9.631803000573209</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2975246528730949</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
+        <v>0.3083678849325592</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.804530396135378</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="n">
         <v>18.02405058424596</v>
       </c>
-      <c r="H6" t="n">
-        <v>0.5974161667792324</v>
-      </c>
       <c r="I6" t="n">
+        <v>0.652767866820271</v>
+      </c>
+      <c r="J6" t="n">
+        <v>13.92147349229983</v>
+      </c>
+      <c r="K6" t="n">
         <v>2.912686349415983</v>
       </c>
-      <c r="J6" t="n">
-        <v>0.2921548949421264</v>
-      </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
+        <v>0.2568417415037383</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2.235569298748505</v>
+      </c>
+      <c r="N6" t="n">
         <v>52.79000399964171</v>
       </c>
-      <c r="L6" t="n">
-        <v>4.467691769428843</v>
+      <c r="O6" t="n">
+        <v>1.37121513926494</v>
+      </c>
+      <c r="P6" t="n">
+        <v>47.73187631198127</v>
       </c>
     </row>
     <row r="7">
@@ -708,26 +788,38 @@
         <v>9.789901513567713</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3039532894150402</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
+        <v>0.5170291484078821</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.376109704298808</v>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="n">
         <v>18.20383718240869</v>
       </c>
-      <c r="H7" t="n">
-        <v>0.5700781010726557</v>
-      </c>
       <c r="I7" t="n">
+        <v>0.6092160685244821</v>
+      </c>
+      <c r="J7" t="n">
+        <v>12.07311562416297</v>
+      </c>
+      <c r="K7" t="n">
         <v>2.985287828596064</v>
       </c>
-      <c r="J7" t="n">
-        <v>0.1936503801153272</v>
-      </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
+        <v>0.2042234060781455</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2.529502188984647</v>
+      </c>
+      <c r="N7" t="n">
         <v>54.3721708206039</v>
       </c>
-      <c r="L7" t="n">
-        <v>1.956391013488016</v>
+      <c r="O7" t="n">
+        <v>3.334700528819338</v>
+      </c>
+      <c r="P7" t="n">
+        <v>47.47747159958216</v>
       </c>
     </row>
     <row r="8">
@@ -748,26 +840,38 @@
         <v>14.94918195657381</v>
       </c>
       <c r="E8" t="n">
-        <v>1.272884943280192</v>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
+        <v>1.694119321374044</v>
+      </c>
+      <c r="F8" t="n">
+        <v>6.217035878164081</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="n">
         <v>23.53428404124674</v>
       </c>
-      <c r="H8" t="n">
-        <v>1.217421950544501</v>
-      </c>
       <c r="I8" t="n">
+        <v>1.478611419389102</v>
+      </c>
+      <c r="J8" t="n">
+        <v>14.15199215348284</v>
+      </c>
+      <c r="K8" t="n">
         <v>4.771704987708077</v>
       </c>
-      <c r="J8" t="n">
-        <v>0.6810150180209344</v>
-      </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
+        <v>0.7096032535990036</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2.406538298692395</v>
+      </c>
+      <c r="N8" t="n">
         <v>102.6347181812276</v>
       </c>
-      <c r="L8" t="n">
-        <v>11.44892790124991</v>
+      <c r="O8" t="n">
+        <v>10.79875824800481</v>
+      </c>
+      <c r="P8" t="n">
+        <v>38.58328398286862</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use tau from HRA
</commit_message>
<xml_diff>
--- a/performance_data/trained/test/metrics.xlsx
+++ b/performance_data/trained/test/metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,67 +446,87 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>rmse_thetass2_spme [milli]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_phie2_spme [mV]</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_if2_spme [mA]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>rmse_vcell_spme [mV]</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_thetass2_hybrid_without_delta [milli]</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_phie2_hybrid_without_delta [mV]</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_if2_hybrid_without_delta [mA]</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_vcell_hybrid_without_delta [mV]</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_thetass2_hybrid [milli]</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_phie2_hybrid [mV]</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_if2_hybrid [mA]</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>rmse_vcell_hybrid [mV]</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>rmse_vcell_hybrid_without_delta [mV]</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_thetass2_hybrid_mtau [milli]</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_phie2_hybrid_mtau [mV]</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_if2_hybrid_mtau [mA]</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>rmse_vcell_hybrid_mtau [mV]</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>rmse_vcell_rom [mV]</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>rmse_thetass2_spme [milli]</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>rmse_thetass2_hybrid [milli]</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>rmse_thetass2_hybrid_without_delta [milli]</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>rmse_phie2_spme [mV]</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>rmse_phie2_hybrid [mV]</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>rmse_phie2_hybrid_without_delta [mV]</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>rmse_if2_spme [mA]</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>rmse_if2_hybrid [mA]</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>rmse_if2_hybrid_without_delta [mA]</t>
         </is>
       </c>
     </row>
@@ -525,42 +545,54 @@
         </is>
       </c>
       <c r="D2" t="n">
+        <v>43.7358703437796</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.978995576824035</v>
+      </c>
+      <c r="F2" t="n">
+        <v>56.67263062870067</v>
+      </c>
+      <c r="G2" t="n">
         <v>18.78470331533877</v>
       </c>
-      <c r="E2" t="n">
-        <v>0.2484402900329776</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1.41983471626149</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
-        <v>43.7358703437796</v>
+        <v>2.293724908164353</v>
       </c>
       <c r="I2" t="n">
-        <v>0.267014520436426</v>
+        <v>0.5341372674866498</v>
       </c>
       <c r="J2" t="n">
-        <v>1.996485785104415</v>
+        <v>4.105678872680572</v>
       </c>
       <c r="K2" t="n">
-        <v>2.978995576824035</v>
+        <v>1.251145118575022</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1915680168484054</v>
+        <v>0.4007139611697978</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9584283649439964</v>
+        <v>0.2897978153470505</v>
       </c>
       <c r="N2" t="n">
-        <v>56.67263062870067</v>
+        <v>1.593423994716917</v>
       </c>
       <c r="O2" t="n">
-        <v>1.986758250353938</v>
+        <v>0.4187197343067486</v>
       </c>
       <c r="P2" t="n">
-        <v>4.853599605237231</v>
-      </c>
+        <v>0.3368233357377967</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.196474083314284</v>
+      </c>
+      <c r="R2" t="n">
+        <v>6.329179078424049</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.3583155051906138</v>
+      </c>
+      <c r="T2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -577,42 +609,54 @@
         </is>
       </c>
       <c r="D3" t="n">
+        <v>15.034764981421</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.2532317906993753</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5.177685837604972</v>
+      </c>
+      <c r="G3" t="n">
         <v>5.003483852125205</v>
       </c>
-      <c r="E3" t="n">
-        <v>0.1992275861903888</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1.683943637335505</v>
-      </c>
-      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>15.034764981421</v>
+        <v>1.203935038555829</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2291191651059691</v>
+        <v>0.4113714936147121</v>
       </c>
       <c r="J3" t="n">
-        <v>1.50508416648509</v>
+        <v>20.62389045872475</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2532317906993753</v>
+        <v>2.30295306187848</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1094559105373297</v>
+        <v>0.2069777797965604</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2673031981268261</v>
+        <v>0.1072690026844791</v>
       </c>
       <c r="N3" t="n">
-        <v>5.177685837604972</v>
+        <v>0.5116107823734578</v>
       </c>
       <c r="O3" t="n">
-        <v>0.5981098243075972</v>
+        <v>0.1344227326742837</v>
       </c>
       <c r="P3" t="n">
-        <v>12.18018861377182</v>
-      </c>
+        <v>0.2283399580241873</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.125320613384622</v>
+      </c>
+      <c r="R3" t="n">
+        <v>1.546829424739875</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.06535990562676323</v>
+      </c>
+      <c r="T3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -629,42 +673,54 @@
         </is>
       </c>
       <c r="D4" t="n">
+        <v>14.87308574524844</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.4996402611546773</v>
+      </c>
+      <c r="F4" t="n">
+        <v>9.120512990525478</v>
+      </c>
+      <c r="G4" t="n">
         <v>4.839307579931836</v>
       </c>
-      <c r="E4" t="n">
-        <v>0.2957377338123012</v>
-      </c>
-      <c r="F4" t="n">
-        <v>2.272985895707731</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>14.87308574524844</v>
+        <v>3.163185622924866</v>
       </c>
       <c r="I4" t="n">
-        <v>0.3188370031423483</v>
+        <v>1.276481120222673</v>
       </c>
       <c r="J4" t="n">
-        <v>2.969493742516178</v>
+        <v>5.427736819300264</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4996402611546773</v>
+        <v>1.276188029148837</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1195641350490709</v>
+        <v>0.2933831423953658</v>
       </c>
       <c r="M4" t="n">
-        <v>1.362948717325113</v>
+        <v>0.07732002857186196</v>
       </c>
       <c r="N4" t="n">
-        <v>9.120512990525478</v>
+        <v>1.36692736406588</v>
       </c>
       <c r="O4" t="n">
-        <v>1.005707166316514</v>
+        <v>0.3322589499956418</v>
       </c>
       <c r="P4" t="n">
-        <v>21.53801454238877</v>
-      </c>
+        <v>0.1338687111506674</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.07512451265799253</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.9090713512831607</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.1371804276628667</v>
+      </c>
+      <c r="T4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -681,42 +737,54 @@
         </is>
       </c>
       <c r="D5" t="n">
+        <v>46.71988130681122</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4.142925913006523</v>
+      </c>
+      <c r="F5" t="n">
+        <v>77.16998448259233</v>
+      </c>
+      <c r="G5" t="n">
         <v>17.3959451475703</v>
       </c>
-      <c r="E5" t="n">
-        <v>4.062989119600359</v>
-      </c>
-      <c r="F5" t="n">
-        <v>7.638299160277519</v>
-      </c>
-      <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
-        <v>46.71988130681122</v>
+        <v>3.569198843582928</v>
       </c>
       <c r="I5" t="n">
-        <v>3.194834529683527</v>
+        <v>0.8915088172082858</v>
       </c>
       <c r="J5" t="n">
-        <v>5.731017690657275</v>
+        <v>100.1547995140992</v>
       </c>
       <c r="K5" t="n">
-        <v>4.142925913006523</v>
+        <v>7.384130577310017</v>
       </c>
       <c r="L5" t="n">
-        <v>0.2663234867236759</v>
+        <v>2.180694896785567</v>
       </c>
       <c r="M5" t="n">
-        <v>5.830591755813333</v>
+        <v>0.3374207023560365</v>
       </c>
       <c r="N5" t="n">
-        <v>77.16998448259233</v>
+        <v>8.577256505218603</v>
       </c>
       <c r="O5" t="n">
-        <v>3.037047053381891</v>
+        <v>1.200392199277645</v>
       </c>
       <c r="P5" t="n">
-        <v>11.25843421902136</v>
-      </c>
+        <v>2.779666701453919</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.2102026984955428</v>
+      </c>
+      <c r="R5" t="n">
+        <v>2.531300974628592</v>
+      </c>
+      <c r="S5" t="n">
+        <v>4.126239001850039</v>
+      </c>
+      <c r="T5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -733,42 +801,54 @@
         </is>
       </c>
       <c r="D6" t="n">
+        <v>18.02405058424596</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.912686349415983</v>
+      </c>
+      <c r="F6" t="n">
+        <v>52.79000399964171</v>
+      </c>
+      <c r="G6" t="n">
         <v>9.631803000573209</v>
       </c>
-      <c r="E6" t="n">
-        <v>0.3083678849325592</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1.804530396135378</v>
-      </c>
-      <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
-        <v>18.02405058424596</v>
+        <v>13.24863715480514</v>
       </c>
       <c r="I6" t="n">
-        <v>0.652767866820271</v>
+        <v>2.019695606016681</v>
       </c>
       <c r="J6" t="n">
-        <v>13.92147349229983</v>
+        <v>40.54638496657045</v>
       </c>
       <c r="K6" t="n">
-        <v>2.912686349415983</v>
+        <v>1.3146297405899</v>
       </c>
       <c r="L6" t="n">
-        <v>0.2568417415037383</v>
+        <v>0.578990546874148</v>
       </c>
       <c r="M6" t="n">
-        <v>2.235569298748505</v>
+        <v>0.1535400392487568</v>
       </c>
       <c r="N6" t="n">
-        <v>52.79000399964171</v>
+        <v>1.566693796553724</v>
       </c>
       <c r="O6" t="n">
-        <v>1.37121513926494</v>
+        <v>0.2424488633090422</v>
       </c>
       <c r="P6" t="n">
-        <v>47.73187631198127</v>
-      </c>
+        <v>0.8536955184065727</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.7135600085984358</v>
+      </c>
+      <c r="R6" t="n">
+        <v>3.642050367788539</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.7065926621248783</v>
+      </c>
+      <c r="T6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -785,42 +865,54 @@
         </is>
       </c>
       <c r="D7" t="n">
+        <v>18.20383718240869</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.985287828596064</v>
+      </c>
+      <c r="F7" t="n">
+        <v>54.3721708206039</v>
+      </c>
+      <c r="G7" t="n">
         <v>9.789901513567713</v>
       </c>
-      <c r="E7" t="n">
-        <v>0.5170291484078821</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3.376109704298808</v>
-      </c>
-      <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>18.20383718240869</v>
+        <v>11.76150623102837</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6092160685244821</v>
+        <v>2.737432530400332</v>
       </c>
       <c r="J7" t="n">
-        <v>12.07311562416297</v>
+        <v>43.35040114086348</v>
       </c>
       <c r="K7" t="n">
-        <v>2.985287828596064</v>
+        <v>3.431444068153565</v>
       </c>
       <c r="L7" t="n">
-        <v>0.2042234060781455</v>
+        <v>0.642965281743617</v>
       </c>
       <c r="M7" t="n">
-        <v>2.529502188984647</v>
+        <v>0.2531807654505578</v>
       </c>
       <c r="N7" t="n">
-        <v>54.3721708206039</v>
+        <v>2.389374947162722</v>
       </c>
       <c r="O7" t="n">
-        <v>3.334700528819338</v>
+        <v>0.3775667471293523</v>
       </c>
       <c r="P7" t="n">
-        <v>47.47747159958216</v>
-      </c>
+        <v>1.46939076461661</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.2291985881086432</v>
+      </c>
+      <c r="R7" t="n">
+        <v>5.982585160341862</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1.111551481148627</v>
+      </c>
+      <c r="T7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -837,42 +929,54 @@
         </is>
       </c>
       <c r="D8" t="n">
+        <v>23.53428404124674</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4.771704987708077</v>
+      </c>
+      <c r="F8" t="n">
+        <v>102.6347181812276</v>
+      </c>
+      <c r="G8" t="n">
         <v>14.94918195657381</v>
       </c>
-      <c r="E8" t="n">
-        <v>1.694119321374044</v>
-      </c>
-      <c r="F8" t="n">
-        <v>6.217035878164081</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>23.53428404124674</v>
+        <v>14.07311921809941</v>
       </c>
       <c r="I8" t="n">
-        <v>1.478611419389102</v>
+        <v>2.0945997301829</v>
       </c>
       <c r="J8" t="n">
-        <v>14.15199215348284</v>
+        <v>40.66663299748471</v>
       </c>
       <c r="K8" t="n">
-        <v>4.771704987708077</v>
+        <v>6.502474003138566</v>
       </c>
       <c r="L8" t="n">
-        <v>0.7096032535990036</v>
+        <v>1.184083850872454</v>
       </c>
       <c r="M8" t="n">
-        <v>2.406538298692395</v>
+        <v>0.7110283462933842</v>
       </c>
       <c r="N8" t="n">
-        <v>102.6347181812276</v>
+        <v>9.798706861476861</v>
       </c>
       <c r="O8" t="n">
-        <v>10.79875824800481</v>
+        <v>1.529324178351341</v>
       </c>
       <c r="P8" t="n">
-        <v>38.58328398286862</v>
-      </c>
+        <v>2.694588622602008</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.8515649338313767</v>
+      </c>
+      <c r="R8" t="n">
+        <v>9.122009511504032</v>
+      </c>
+      <c r="S8" t="n">
+        <v>2.262576439384274</v>
+      </c>
+      <c r="T8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>